<commit_message>
[FIX] Seleção de anexos: navegação na tela de anexos agora é feita utilizando o teclado ao invés de clicks para evitar problema de seletor.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_RequestIt\PROD\dhl-dtentry-requestit_2.3.21\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_RequestIt\HML\dhl-dtentry-requestit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F0BB55-8163-496C-A609-18DE39BCB935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CAE287-8AA9-4489-892A-C4233D4A20C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
     <t>emailXML_CARGA</t>
   </si>
   <si>
-    <t>CARGA</t>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
   <dimension ref="A1:Z1030"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4764,4 +4764,10 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{736915f3-2f02-4945-8997-f2963298db46}" enabled="1" method="Standard" siteId="{cd99fef8-1cd3-4a2a-9bdf-15531181d65e}" contentBits="1" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[FIX] 21/11/2024: Tratativa para novo pop-up
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_RequestIt\PROD\dhl-dtentry-requestit\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_RequestIt\PROD\dhl-dtentry-download-requestit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A7DC4E-1D35-4CE2-9772-3B4F7B147B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4759BEE-B9CA-47B3-AB3E-0E68C042DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
     <t>emailXML_CARGA</t>
   </si>
   <si>
-    <t>PROD</t>
+    <t>CARGA</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
   <dimension ref="A1:Z1030"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>